<commit_message>
added user ads status filters template, little work on user ads controller, updated self evaluation protocol
</commit_message>
<xml_diff>
--- a/Ads/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -391,10 +391,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -670,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:E33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,11 +745,11 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -784,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
@@ -867,7 +867,9 @@
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5">
+        <v>5</v>
+      </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
@@ -877,7 +879,9 @@
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5">
+        <v>10</v>
+      </c>
       <c r="D19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1201,7 +1205,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
started work on user ads edit/delete
</commit_message>
<xml_diff>
--- a/Ads/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -670,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +901,9 @@
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
@@ -911,7 +913,9 @@
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5">
+        <v>5</v>
+      </c>
       <c r="D22" s="5" t="s">
         <v>5</v>
       </c>
@@ -921,7 +925,9 @@
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5">
+        <v>5</v>
+      </c>
       <c r="D23" s="5" t="s">
         <v>5</v>
       </c>
@@ -931,7 +937,9 @@
       <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
       <c r="D24" s="5" t="s">
         <v>5</v>
       </c>
@@ -941,7 +949,9 @@
       <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
       <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
@@ -1205,7 +1215,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
Ad deletion implemented, updated self evaluation protocol
</commit_message>
<xml_diff>
--- a/Ads/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -670,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +961,9 @@
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5">
+        <v>5</v>
+      </c>
       <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
@@ -981,7 +983,9 @@
       <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
       <c r="D28" s="5" t="s">
         <v>5</v>
       </c>
@@ -1215,7 +1219,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
implemented password changing, updated self-evaluation protocol
</commit_message>
<xml_diff>
--- a/Ads/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -192,13 +192,13 @@
     <t>∞</t>
   </si>
   <si>
-    <t>Hpetrov</t>
-  </si>
-  <si>
     <t>Hristo Petrov</t>
   </si>
   <si>
     <t>https://github.com/Razhagal</t>
+  </si>
+  <si>
+    <t>HPetrov</t>
   </si>
 </sst>
 </file>
@@ -670,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +718,7 @@
         <v>51</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -728,7 +728,7 @@
         <v>53</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -746,7 +746,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -755,7 +755,9 @@
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <v>7</v>
+      </c>
       <c r="D8" s="12" t="s">
         <v>56</v>
       </c>
@@ -765,7 +767,9 @@
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>34</v>
+      </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
       </c>
@@ -995,7 +999,9 @@
       <c r="B29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="5">
+        <v>5</v>
+      </c>
       <c r="D29" s="5" t="s">
         <v>5</v>
       </c>
@@ -1005,7 +1011,9 @@
       <c r="B30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5">
+        <v>5</v>
+      </c>
       <c r="D30" s="5" t="s">
         <v>5</v>
       </c>
@@ -1219,7 +1227,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
added some password check and notifications
</commit_message>
<xml_diff>
--- a/Ads/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/Ads/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -670,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -681,7 +681,7 @@
   <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B10" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>